<commit_message>
Docs + Upgraded Excel etc.
</commit_message>
<xml_diff>
--- a/Excel/Excel.xlsx
+++ b/Excel/Excel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yigitemre/Desktop/6838scout/Excel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yigit\Desktop\ScoutingApp6838\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8970125-F3DB-2A46-8367-21544B92196C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9821CF57-702F-4D62-B17E-93941376B362}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{A46E49DD-D669-429F-AA31-B068C359770D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A46E49DD-D669-429F-AA31-B068C359770D}"/>
   </bookViews>
   <sheets>
     <sheet name="Insert" sheetId="1" r:id="rId1"/>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="30">
   <si>
     <t>Scouter</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -151,12 +151,15 @@
   <si>
     <t>Team</t>
   </si>
+  <si>
+    <t>s=Yiğit Emre Çulcuoğlu;e=2022 İzmir Regional;l=f;m=1;r=b2;t=6838;as=[54];at=Y;au=8;al=3;ac=Y;tu=5;tl=6;tm=1;tn=2;wd=Y;cl=b;ss=[53,56,44,58,34,20,17,18,41,51,51,16,26,50,64,68,34];c=4;be=Y;cn=1;ds=v;dr=v;d=N;to=N;cf=N;co=Commen</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -291,7 +294,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Teması">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -590,16 +593,16 @@
   <dimension ref="A1:AP70"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="20.6640625" customWidth="1"/>
-    <col min="2" max="29" width="10.6640625" customWidth="1"/>
+    <col min="1" max="1" width="20.7109375" customWidth="1"/>
+    <col min="2" max="29" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:42">
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
@@ -691,7 +694,7 @@
       <c r="AJ1" s="3"/>
       <c r="AK1" s="3"/>
     </row>
-    <row r="2" spans="1:42" ht="20" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:42" ht="20.25">
       <c r="A2" s="6" t="s">
         <v>6</v>
       </c>
@@ -817,7 +820,7 @@
       <c r="AO2" s="4"/>
       <c r="AP2" s="4"/>
     </row>
-    <row r="3" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:42">
       <c r="B3" s="1" t="str" cm="1">
         <f t="array" aca="1" ref="B3" ca="1">TRANSPOSE(TRIM(MID(SUBSTITUTE(";"&amp;A3,";",REPT(" ",LEN(A3)+1)),ROW(INDIRECT("A1:A"&amp;LEN(A3)-LEN(SUBSTITUTE(A3,";",""))+1))*LEN(A3)+1,LEN(A3)+1)))</f>
         <v/>
@@ -862,37 +865,118 @@
       <c r="AO3" s="4"/>
       <c r="AP3" s="4"/>
     </row>
-    <row r="4" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:42">
+      <c r="A4" t="s">
+        <v>29</v>
+      </c>
       <c r="B4" s="1" t="str" cm="1">
-        <f t="array" aca="1" ref="B4" ca="1">TRANSPOSE(TRIM(MID(SUBSTITUTE(";"&amp;A4,";",REPT(" ",LEN(A4)+1)),ROW(INDIRECT("A1:A"&amp;LEN(A4)-LEN(SUBSTITUTE(A4,";",""))+1))*LEN(A4)+1,LEN(A4)+1)))</f>
-        <v/>
-      </c>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
-      <c r="L4" s="1"/>
-      <c r="M4" s="1"/>
-      <c r="N4" s="1"/>
-      <c r="O4" s="1"/>
-      <c r="P4" s="1"/>
-      <c r="Q4" s="1"/>
-      <c r="R4" s="1"/>
-      <c r="S4" s="1"/>
-      <c r="T4" s="1"/>
-      <c r="U4" s="1"/>
-      <c r="V4" s="1"/>
-      <c r="W4" s="1"/>
-      <c r="X4" s="1"/>
-      <c r="Y4" s="1"/>
-      <c r="Z4" s="1"/>
-      <c r="AA4" s="1"/>
-      <c r="AB4" s="1"/>
+        <f t="array" aca="1" ref="B4:AB4" ca="1">TRANSPOSE(TRIM(MID(SUBSTITUTE(";"&amp;A4,";",REPT(" ",LEN(A4)+1)),ROW(INDIRECT("A1:A"&amp;LEN(A4)-LEN(SUBSTITUTE(A4,";",""))+1))*LEN(A4)+1,LEN(A4)+1)))</f>
+        <v>s=Yiğit Emre Çulcuoğlu</v>
+      </c>
+      <c r="C4" s="1" t="str">
+        <f ca="1"/>
+        <v>e=2022 İzmir Regional</v>
+      </c>
+      <c r="D4" s="1" t="str">
+        <f ca="1"/>
+        <v>l=f</v>
+      </c>
+      <c r="E4" s="1" t="str">
+        <f ca="1"/>
+        <v>m=1</v>
+      </c>
+      <c r="F4" s="1" t="str">
+        <f ca="1"/>
+        <v>r=b2</v>
+      </c>
+      <c r="G4" s="1" t="str">
+        <f ca="1"/>
+        <v>t=6838</v>
+      </c>
+      <c r="H4" s="1" t="str">
+        <f ca="1"/>
+        <v>as=[54]</v>
+      </c>
+      <c r="I4" s="1" t="str">
+        <f ca="1"/>
+        <v>at=Y</v>
+      </c>
+      <c r="J4" s="1" t="str">
+        <f ca="1"/>
+        <v>au=8</v>
+      </c>
+      <c r="K4" s="1" t="str">
+        <f ca="1"/>
+        <v>al=3</v>
+      </c>
+      <c r="L4" s="1" t="str">
+        <f ca="1"/>
+        <v>ac=Y</v>
+      </c>
+      <c r="M4" s="1" t="str">
+        <f ca="1"/>
+        <v>tu=5</v>
+      </c>
+      <c r="N4" s="1" t="str">
+        <f ca="1"/>
+        <v>tl=6</v>
+      </c>
+      <c r="O4" s="1" t="str">
+        <f ca="1"/>
+        <v>tm=1</v>
+      </c>
+      <c r="P4" s="1" t="str">
+        <f ca="1"/>
+        <v>tn=2</v>
+      </c>
+      <c r="Q4" s="1" t="str">
+        <f ca="1"/>
+        <v>wd=Y</v>
+      </c>
+      <c r="R4" s="1" t="str">
+        <f ca="1"/>
+        <v>cl=b</v>
+      </c>
+      <c r="S4" s="1" t="str">
+        <f ca="1"/>
+        <v>ss=[53,56,44,58,34,20,17,18,41,51,51,16,26,50,64,68,34]</v>
+      </c>
+      <c r="T4" s="1" t="str">
+        <f ca="1"/>
+        <v>c=4</v>
+      </c>
+      <c r="U4" s="1" t="str">
+        <f ca="1"/>
+        <v>be=Y</v>
+      </c>
+      <c r="V4" s="1" t="str">
+        <f ca="1"/>
+        <v>cn=1</v>
+      </c>
+      <c r="W4" s="1" t="str">
+        <f ca="1"/>
+        <v>ds=v</v>
+      </c>
+      <c r="X4" s="1" t="str">
+        <f ca="1"/>
+        <v>dr=v</v>
+      </c>
+      <c r="Y4" s="1" t="str">
+        <f ca="1"/>
+        <v>d=N</v>
+      </c>
+      <c r="Z4" s="1" t="str">
+        <f ca="1"/>
+        <v>to=N</v>
+      </c>
+      <c r="AA4" s="1" t="str">
+        <f ca="1"/>
+        <v>cf=N</v>
+      </c>
+      <c r="AB4" s="1" t="str">
+        <f ca="1"/>
+        <v>co=Commen</v>
+      </c>
       <c r="AC4" s="1"/>
       <c r="AD4" s="4"/>
       <c r="AE4" s="4"/>
@@ -907,7 +991,7 @@
       <c r="AO4" s="4"/>
       <c r="AP4" s="4"/>
     </row>
-    <row r="5" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:42">
       <c r="B5" s="1" t="str" cm="1">
         <f t="array" aca="1" ref="B5" ca="1">TRANSPOSE(TRIM(MID(SUBSTITUTE(";"&amp;A5,";",REPT(" ",LEN(A5)+1)),ROW(INDIRECT("A1:A"&amp;LEN(A5)-LEN(SUBSTITUTE(A5,";",""))+1))*LEN(A5)+1,LEN(A5)+1)))</f>
         <v/>
@@ -952,7 +1036,7 @@
       <c r="AO5" s="4"/>
       <c r="AP5" s="4"/>
     </row>
-    <row r="6" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:42">
       <c r="B6" s="1" t="str" cm="1">
         <f t="array" aca="1" ref="B6" ca="1">TRANSPOSE(TRIM(MID(SUBSTITUTE(";"&amp;A6,";",REPT(" ",LEN(A6)+1)),ROW(INDIRECT("A1:A"&amp;LEN(A6)-LEN(SUBSTITUTE(A6,";",""))+1))*LEN(A6)+1,LEN(A6)+1)))</f>
         <v/>
@@ -997,7 +1081,7 @@
       <c r="AO6" s="4"/>
       <c r="AP6" s="4"/>
     </row>
-    <row r="7" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:42">
       <c r="B7" s="1" t="str" cm="1">
         <f t="array" aca="1" ref="B7" ca="1">TRANSPOSE(TRIM(MID(SUBSTITUTE(";"&amp;A7,";",REPT(" ",LEN(A7)+1)),ROW(INDIRECT("A1:A"&amp;LEN(A7)-LEN(SUBSTITUTE(A7,";",""))+1))*LEN(A7)+1,LEN(A7)+1)))</f>
         <v/>
@@ -1042,7 +1126,7 @@
       <c r="AO7" s="4"/>
       <c r="AP7" s="4"/>
     </row>
-    <row r="8" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:42">
       <c r="B8" s="1" t="str" cm="1">
         <f t="array" aca="1" ref="B8" ca="1">TRANSPOSE(TRIM(MID(SUBSTITUTE(";"&amp;A8,";",REPT(" ",LEN(A8)+1)),ROW(INDIRECT("A1:A"&amp;LEN(A8)-LEN(SUBSTITUTE(A8,";",""))+1))*LEN(A8)+1,LEN(A8)+1)))</f>
         <v/>
@@ -1087,7 +1171,7 @@
       <c r="AO8" s="4"/>
       <c r="AP8" s="4"/>
     </row>
-    <row r="9" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:42">
       <c r="B9" s="1" t="str" cm="1">
         <f t="array" aca="1" ref="B9" ca="1">TRANSPOSE(TRIM(MID(SUBSTITUTE(";"&amp;A9,";",REPT(" ",LEN(A9)+1)),ROW(INDIRECT("A1:A"&amp;LEN(A9)-LEN(SUBSTITUTE(A9,";",""))+1))*LEN(A9)+1,LEN(A9)+1)))</f>
         <v/>
@@ -1132,7 +1216,7 @@
       <c r="AO9" s="4"/>
       <c r="AP9" s="4"/>
     </row>
-    <row r="10" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:42">
       <c r="B10" s="1" t="str" cm="1">
         <f t="array" aca="1" ref="B10" ca="1">TRANSPOSE(TRIM(MID(SUBSTITUTE(";"&amp;A10,";",REPT(" ",LEN(A10)+1)),ROW(INDIRECT("A1:A"&amp;LEN(A10)-LEN(SUBSTITUTE(A10,";",""))+1))*LEN(A10)+1,LEN(A10)+1)))</f>
         <v/>
@@ -1177,7 +1261,7 @@
       <c r="AO10" s="4"/>
       <c r="AP10" s="4"/>
     </row>
-    <row r="11" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:42">
       <c r="B11" s="1" t="str" cm="1">
         <f t="array" aca="1" ref="B11" ca="1">TRANSPOSE(TRIM(MID(SUBSTITUTE(";"&amp;A11,";",REPT(" ",LEN(A11)+1)),ROW(INDIRECT("A1:A"&amp;LEN(A11)-LEN(SUBSTITUTE(A11,";",""))+1))*LEN(A11)+1,LEN(A11)+1)))</f>
         <v/>
@@ -1222,7 +1306,7 @@
       <c r="AO11" s="4"/>
       <c r="AP11" s="4"/>
     </row>
-    <row r="12" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:42">
       <c r="B12" s="1" t="str" cm="1">
         <f t="array" aca="1" ref="B12" ca="1">TRANSPOSE(TRIM(MID(SUBSTITUTE(";"&amp;A12,";",REPT(" ",LEN(A12)+1)),ROW(INDIRECT("A1:A"&amp;LEN(A12)-LEN(SUBSTITUTE(A12,";",""))+1))*LEN(A12)+1,LEN(A12)+1)))</f>
         <v/>
@@ -1267,7 +1351,7 @@
       <c r="AO12" s="4"/>
       <c r="AP12" s="4"/>
     </row>
-    <row r="13" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:42">
       <c r="B13" s="1" t="str" cm="1">
         <f t="array" aca="1" ref="B13" ca="1">TRANSPOSE(TRIM(MID(SUBSTITUTE(";"&amp;A13,";",REPT(" ",LEN(A13)+1)),ROW(INDIRECT("A1:A"&amp;LEN(A13)-LEN(SUBSTITUTE(A13,";",""))+1))*LEN(A13)+1,LEN(A13)+1)))</f>
         <v/>
@@ -1312,7 +1396,7 @@
       <c r="AO13" s="4"/>
       <c r="AP13" s="4"/>
     </row>
-    <row r="14" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:42">
       <c r="B14" s="1" t="str" cm="1">
         <f t="array" aca="1" ref="B14" ca="1">TRANSPOSE(TRIM(MID(SUBSTITUTE(";"&amp;A14,";",REPT(" ",LEN(A14)+1)),ROW(INDIRECT("A1:A"&amp;LEN(A14)-LEN(SUBSTITUTE(A14,";",""))+1))*LEN(A14)+1,LEN(A14)+1)))</f>
         <v/>
@@ -1357,7 +1441,7 @@
       <c r="AO14" s="4"/>
       <c r="AP14" s="4"/>
     </row>
-    <row r="15" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:42">
       <c r="B15" s="1" t="str" cm="1">
         <f t="array" aca="1" ref="B15" ca="1">TRANSPOSE(TRIM(MID(SUBSTITUTE(";"&amp;A15,";",REPT(" ",LEN(A15)+1)),ROW(INDIRECT("A1:A"&amp;LEN(A15)-LEN(SUBSTITUTE(A15,";",""))+1))*LEN(A15)+1,LEN(A15)+1)))</f>
         <v/>
@@ -1402,7 +1486,7 @@
       <c r="AO15" s="4"/>
       <c r="AP15" s="4"/>
     </row>
-    <row r="16" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:42">
       <c r="B16" s="1" t="str" cm="1">
         <f t="array" aca="1" ref="B16" ca="1">TRANSPOSE(TRIM(MID(SUBSTITUTE(";"&amp;A16,";",REPT(" ",LEN(A16)+1)),ROW(INDIRECT("A1:A"&amp;LEN(A16)-LEN(SUBSTITUTE(A16,";",""))+1))*LEN(A16)+1,LEN(A16)+1)))</f>
         <v/>
@@ -1447,7 +1531,7 @@
       <c r="AO16" s="4"/>
       <c r="AP16" s="4"/>
     </row>
-    <row r="17" spans="2:42" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:42">
       <c r="B17" s="1" t="str" cm="1">
         <f t="array" aca="1" ref="B17" ca="1">TRANSPOSE(TRIM(MID(SUBSTITUTE(";"&amp;A17,";",REPT(" ",LEN(A17)+1)),ROW(INDIRECT("A1:A"&amp;LEN(A17)-LEN(SUBSTITUTE(A17,";",""))+1))*LEN(A17)+1,LEN(A17)+1)))</f>
         <v/>
@@ -1492,7 +1576,7 @@
       <c r="AO17" s="4"/>
       <c r="AP17" s="4"/>
     </row>
-    <row r="18" spans="2:42" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:42">
       <c r="B18" s="1" t="str" cm="1">
         <f t="array" aca="1" ref="B18" ca="1">TRANSPOSE(TRIM(MID(SUBSTITUTE(";"&amp;A18,";",REPT(" ",LEN(A18)+1)),ROW(INDIRECT("A1:A"&amp;LEN(A18)-LEN(SUBSTITUTE(A18,";",""))+1))*LEN(A18)+1,LEN(A18)+1)))</f>
         <v/>
@@ -1537,7 +1621,7 @@
       <c r="AO18" s="4"/>
       <c r="AP18" s="4"/>
     </row>
-    <row r="19" spans="2:42" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:42">
       <c r="B19" s="1" t="str" cm="1">
         <f t="array" aca="1" ref="B19" ca="1">TRANSPOSE(TRIM(MID(SUBSTITUTE(";"&amp;A19,";",REPT(" ",LEN(A19)+1)),ROW(INDIRECT("A1:A"&amp;LEN(A19)-LEN(SUBSTITUTE(A19,";",""))+1))*LEN(A19)+1,LEN(A19)+1)))</f>
         <v/>
@@ -1582,7 +1666,7 @@
       <c r="AO19" s="4"/>
       <c r="AP19" s="4"/>
     </row>
-    <row r="20" spans="2:42" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:42">
       <c r="B20" s="1" t="str" cm="1">
         <f t="array" aca="1" ref="B20" ca="1">TRANSPOSE(TRIM(MID(SUBSTITUTE(";"&amp;A20,";",REPT(" ",LEN(A20)+1)),ROW(INDIRECT("A1:A"&amp;LEN(A20)-LEN(SUBSTITUTE(A20,";",""))+1))*LEN(A20)+1,LEN(A20)+1)))</f>
         <v/>
@@ -1615,7 +1699,7 @@
       <c r="AB20" s="1"/>
       <c r="AC20" s="1"/>
     </row>
-    <row r="21" spans="2:42" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:42">
       <c r="B21" s="1" t="str" cm="1">
         <f t="array" aca="1" ref="B21" ca="1">TRANSPOSE(TRIM(MID(SUBSTITUTE(";"&amp;A21,";",REPT(" ",LEN(A21)+1)),ROW(INDIRECT("A1:A"&amp;LEN(A21)-LEN(SUBSTITUTE(A21,";",""))+1))*LEN(A21)+1,LEN(A21)+1)))</f>
         <v/>
@@ -1648,7 +1732,7 @@
       <c r="AB21" s="1"/>
       <c r="AC21" s="1"/>
     </row>
-    <row r="22" spans="2:42" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:42">
       <c r="B22" s="1" t="str" cm="1">
         <f t="array" aca="1" ref="B22" ca="1">TRANSPOSE(TRIM(MID(SUBSTITUTE(";"&amp;A22,";",REPT(" ",LEN(A22)+1)),ROW(INDIRECT("A1:A"&amp;LEN(A22)-LEN(SUBSTITUTE(A22,";",""))+1))*LEN(A22)+1,LEN(A22)+1)))</f>
         <v/>
@@ -1681,7 +1765,7 @@
       <c r="AB22" s="1"/>
       <c r="AC22" s="1"/>
     </row>
-    <row r="23" spans="2:42" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:42">
       <c r="B23" s="1" t="str" cm="1">
         <f t="array" aca="1" ref="B23" ca="1">TRANSPOSE(TRIM(MID(SUBSTITUTE(";"&amp;A23,";",REPT(" ",LEN(A23)+1)),ROW(INDIRECT("A1:A"&amp;LEN(A23)-LEN(SUBSTITUTE(A23,";",""))+1))*LEN(A23)+1,LEN(A23)+1)))</f>
         <v/>
@@ -1714,7 +1798,7 @@
       <c r="AB23" s="1"/>
       <c r="AC23" s="1"/>
     </row>
-    <row r="24" spans="2:42" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:42">
       <c r="B24" s="1" t="str" cm="1">
         <f t="array" aca="1" ref="B24" ca="1">TRANSPOSE(TRIM(MID(SUBSTITUTE(";"&amp;A24,";",REPT(" ",LEN(A24)+1)),ROW(INDIRECT("A1:A"&amp;LEN(A24)-LEN(SUBSTITUTE(A24,";",""))+1))*LEN(A24)+1,LEN(A24)+1)))</f>
         <v/>
@@ -1747,7 +1831,7 @@
       <c r="AB24" s="1"/>
       <c r="AC24" s="1"/>
     </row>
-    <row r="25" spans="2:42" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:42">
       <c r="B25" s="1" t="str" cm="1">
         <f t="array" aca="1" ref="B25" ca="1">TRANSPOSE(TRIM(MID(SUBSTITUTE(";"&amp;A25,";",REPT(" ",LEN(A25)+1)),ROW(INDIRECT("A1:A"&amp;LEN(A25)-LEN(SUBSTITUTE(A25,";",""))+1))*LEN(A25)+1,LEN(A25)+1)))</f>
         <v/>
@@ -1780,7 +1864,7 @@
       <c r="AB25" s="1"/>
       <c r="AC25" s="1"/>
     </row>
-    <row r="26" spans="2:42" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:42">
       <c r="B26" s="1" t="str" cm="1">
         <f t="array" aca="1" ref="B26" ca="1">TRANSPOSE(TRIM(MID(SUBSTITUTE(";"&amp;A26,";",REPT(" ",LEN(A26)+1)),ROW(INDIRECT("A1:A"&amp;LEN(A26)-LEN(SUBSTITUTE(A26,";",""))+1))*LEN(A26)+1,LEN(A26)+1)))</f>
         <v/>
@@ -1813,7 +1897,7 @@
       <c r="AB26" s="1"/>
       <c r="AC26" s="1"/>
     </row>
-    <row r="27" spans="2:42" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:42">
       <c r="B27" s="1" t="str" cm="1">
         <f t="array" aca="1" ref="B27" ca="1">TRANSPOSE(TRIM(MID(SUBSTITUTE(";"&amp;A27,";",REPT(" ",LEN(A27)+1)),ROW(INDIRECT("A1:A"&amp;LEN(A27)-LEN(SUBSTITUTE(A27,";",""))+1))*LEN(A27)+1,LEN(A27)+1)))</f>
         <v/>
@@ -1846,7 +1930,7 @@
       <c r="AB27" s="1"/>
       <c r="AC27" s="1"/>
     </row>
-    <row r="28" spans="2:42" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:42">
       <c r="B28" s="1" t="str" cm="1">
         <f t="array" aca="1" ref="B28" ca="1">TRANSPOSE(TRIM(MID(SUBSTITUTE(";"&amp;A28,";",REPT(" ",LEN(A28)+1)),ROW(INDIRECT("A1:A"&amp;LEN(A28)-LEN(SUBSTITUTE(A28,";",""))+1))*LEN(A28)+1,LEN(A28)+1)))</f>
         <v/>
@@ -1879,7 +1963,7 @@
       <c r="AB28" s="1"/>
       <c r="AC28" s="1"/>
     </row>
-    <row r="29" spans="2:42" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:42">
       <c r="B29" s="1" t="str" cm="1">
         <f t="array" aca="1" ref="B29" ca="1">TRANSPOSE(TRIM(MID(SUBSTITUTE(";"&amp;A29,";",REPT(" ",LEN(A29)+1)),ROW(INDIRECT("A1:A"&amp;LEN(A29)-LEN(SUBSTITUTE(A29,";",""))+1))*LEN(A29)+1,LEN(A29)+1)))</f>
         <v/>
@@ -1912,7 +1996,7 @@
       <c r="AB29" s="1"/>
       <c r="AC29" s="1"/>
     </row>
-    <row r="30" spans="2:42" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:42">
       <c r="B30" s="1" t="str" cm="1">
         <f t="array" aca="1" ref="B30" ca="1">TRANSPOSE(TRIM(MID(SUBSTITUTE(";"&amp;A30,";",REPT(" ",LEN(A30)+1)),ROW(INDIRECT("A1:A"&amp;LEN(A30)-LEN(SUBSTITUTE(A30,";",""))+1))*LEN(A30)+1,LEN(A30)+1)))</f>
         <v/>
@@ -1945,7 +2029,7 @@
       <c r="AB30" s="1"/>
       <c r="AC30" s="1"/>
     </row>
-    <row r="31" spans="2:42" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:42">
       <c r="B31" s="1" t="str" cm="1">
         <f t="array" aca="1" ref="B31" ca="1">TRANSPOSE(TRIM(MID(SUBSTITUTE(";"&amp;A31,";",REPT(" ",LEN(A31)+1)),ROW(INDIRECT("A1:A"&amp;LEN(A31)-LEN(SUBSTITUTE(A31,";",""))+1))*LEN(A31)+1,LEN(A31)+1)))</f>
         <v/>
@@ -1978,7 +2062,7 @@
       <c r="AB31" s="1"/>
       <c r="AC31" s="1"/>
     </row>
-    <row r="32" spans="2:42" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:42">
       <c r="B32" s="1" t="str" cm="1">
         <f t="array" aca="1" ref="B32" ca="1">TRANSPOSE(TRIM(MID(SUBSTITUTE(";"&amp;A32,";",REPT(" ",LEN(A32)+1)),ROW(INDIRECT("A1:A"&amp;LEN(A32)-LEN(SUBSTITUTE(A32,";",""))+1))*LEN(A32)+1,LEN(A32)+1)))</f>
         <v/>
@@ -2011,7 +2095,7 @@
       <c r="AB32" s="1"/>
       <c r="AC32" s="1"/>
     </row>
-    <row r="33" spans="2:29" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:29">
       <c r="B33" s="1" t="str" cm="1">
         <f t="array" aca="1" ref="B33" ca="1">TRANSPOSE(TRIM(MID(SUBSTITUTE(";"&amp;A33,";",REPT(" ",LEN(A33)+1)),ROW(INDIRECT("A1:A"&amp;LEN(A33)-LEN(SUBSTITUTE(A33,";",""))+1))*LEN(A33)+1,LEN(A33)+1)))</f>
         <v/>
@@ -2044,7 +2128,7 @@
       <c r="AB33" s="1"/>
       <c r="AC33" s="1"/>
     </row>
-    <row r="34" spans="2:29" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:29">
       <c r="B34" s="1" t="str" cm="1">
         <f t="array" aca="1" ref="B34" ca="1">TRANSPOSE(TRIM(MID(SUBSTITUTE(";"&amp;A34,";",REPT(" ",LEN(A34)+1)),ROW(INDIRECT("A1:A"&amp;LEN(A34)-LEN(SUBSTITUTE(A34,";",""))+1))*LEN(A34)+1,LEN(A34)+1)))</f>
         <v/>
@@ -2077,7 +2161,7 @@
       <c r="AB34" s="1"/>
       <c r="AC34" s="1"/>
     </row>
-    <row r="35" spans="2:29" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:29">
       <c r="B35" s="1" t="str" cm="1">
         <f t="array" aca="1" ref="B35" ca="1">TRANSPOSE(TRIM(MID(SUBSTITUTE(";"&amp;A35,";",REPT(" ",LEN(A35)+1)),ROW(INDIRECT("A1:A"&amp;LEN(A35)-LEN(SUBSTITUTE(A35,";",""))+1))*LEN(A35)+1,LEN(A35)+1)))</f>
         <v/>
@@ -2110,7 +2194,7 @@
       <c r="AB35" s="1"/>
       <c r="AC35" s="1"/>
     </row>
-    <row r="36" spans="2:29" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:29">
       <c r="B36" s="1" t="str" cm="1">
         <f t="array" aca="1" ref="B36" ca="1">TRANSPOSE(TRIM(MID(SUBSTITUTE(";"&amp;A36,";",REPT(" ",LEN(A36)+1)),ROW(INDIRECT("A1:A"&amp;LEN(A36)-LEN(SUBSTITUTE(A36,";",""))+1))*LEN(A36)+1,LEN(A36)+1)))</f>
         <v/>
@@ -2143,7 +2227,7 @@
       <c r="AB36" s="1"/>
       <c r="AC36" s="1"/>
     </row>
-    <row r="37" spans="2:29" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:29">
       <c r="B37" s="1" t="str" cm="1">
         <f t="array" aca="1" ref="B37" ca="1">TRANSPOSE(TRIM(MID(SUBSTITUTE(";"&amp;A37,";",REPT(" ",LEN(A37)+1)),ROW(INDIRECT("A1:A"&amp;LEN(A37)-LEN(SUBSTITUTE(A37,";",""))+1))*LEN(A37)+1,LEN(A37)+1)))</f>
         <v/>
@@ -2176,7 +2260,7 @@
       <c r="AB37" s="1"/>
       <c r="AC37" s="1"/>
     </row>
-    <row r="38" spans="2:29" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:29">
       <c r="B38" s="1" t="str" cm="1">
         <f t="array" aca="1" ref="B38" ca="1">TRANSPOSE(TRIM(MID(SUBSTITUTE(";"&amp;A38,";",REPT(" ",LEN(A38)+1)),ROW(INDIRECT("A1:A"&amp;LEN(A38)-LEN(SUBSTITUTE(A38,";",""))+1))*LEN(A38)+1,LEN(A38)+1)))</f>
         <v/>
@@ -2209,7 +2293,7 @@
       <c r="AB38" s="1"/>
       <c r="AC38" s="1"/>
     </row>
-    <row r="39" spans="2:29" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:29">
       <c r="B39" s="1" t="str" cm="1">
         <f t="array" aca="1" ref="B39" ca="1">TRANSPOSE(TRIM(MID(SUBSTITUTE(";"&amp;A39,";",REPT(" ",LEN(A39)+1)),ROW(INDIRECT("A1:A"&amp;LEN(A39)-LEN(SUBSTITUTE(A39,";",""))+1))*LEN(A39)+1,LEN(A39)+1)))</f>
         <v/>
@@ -2242,7 +2326,7 @@
       <c r="AB39" s="1"/>
       <c r="AC39" s="1"/>
     </row>
-    <row r="40" spans="2:29" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:29">
       <c r="B40" s="1" t="str" cm="1">
         <f t="array" aca="1" ref="B40" ca="1">TRANSPOSE(TRIM(MID(SUBSTITUTE(";"&amp;A40,";",REPT(" ",LEN(A40)+1)),ROW(INDIRECT("A1:A"&amp;LEN(A40)-LEN(SUBSTITUTE(A40,";",""))+1))*LEN(A40)+1,LEN(A40)+1)))</f>
         <v/>
@@ -2275,7 +2359,7 @@
       <c r="AB40" s="1"/>
       <c r="AC40" s="1"/>
     </row>
-    <row r="41" spans="2:29" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:29">
       <c r="B41" s="1" t="str" cm="1">
         <f t="array" aca="1" ref="B41" ca="1">TRANSPOSE(TRIM(MID(SUBSTITUTE(";"&amp;A41,";",REPT(" ",LEN(A41)+1)),ROW(INDIRECT("A1:A"&amp;LEN(A41)-LEN(SUBSTITUTE(A41,";",""))+1))*LEN(A41)+1,LEN(A41)+1)))</f>
         <v/>
@@ -2308,7 +2392,7 @@
       <c r="AB41" s="1"/>
       <c r="AC41" s="1"/>
     </row>
-    <row r="42" spans="2:29" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:29">
       <c r="B42" s="1" t="str" cm="1">
         <f t="array" aca="1" ref="B42" ca="1">TRANSPOSE(TRIM(MID(SUBSTITUTE(";"&amp;A42,";",REPT(" ",LEN(A42)+1)),ROW(INDIRECT("A1:A"&amp;LEN(A42)-LEN(SUBSTITUTE(A42,";",""))+1))*LEN(A42)+1,LEN(A42)+1)))</f>
         <v/>
@@ -2341,7 +2425,7 @@
       <c r="AB42" s="1"/>
       <c r="AC42" s="1"/>
     </row>
-    <row r="43" spans="2:29" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:29">
       <c r="B43" s="1" t="str" cm="1">
         <f t="array" aca="1" ref="B43" ca="1">TRANSPOSE(TRIM(MID(SUBSTITUTE(";"&amp;A43,";",REPT(" ",LEN(A43)+1)),ROW(INDIRECT("A1:A"&amp;LEN(A43)-LEN(SUBSTITUTE(A43,";",""))+1))*LEN(A43)+1,LEN(A43)+1)))</f>
         <v/>
@@ -2374,7 +2458,7 @@
       <c r="AB43" s="1"/>
       <c r="AC43" s="1"/>
     </row>
-    <row r="44" spans="2:29" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:29">
       <c r="B44" s="1" t="str" cm="1">
         <f t="array" aca="1" ref="B44" ca="1">TRANSPOSE(TRIM(MID(SUBSTITUTE(";"&amp;A44,";",REPT(" ",LEN(A44)+1)),ROW(INDIRECT("A1:A"&amp;LEN(A44)-LEN(SUBSTITUTE(A44,";",""))+1))*LEN(A44)+1,LEN(A44)+1)))</f>
         <v/>
@@ -2407,7 +2491,7 @@
       <c r="AB44" s="1"/>
       <c r="AC44" s="1"/>
     </row>
-    <row r="45" spans="2:29" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:29">
       <c r="B45" s="1" t="str" cm="1">
         <f t="array" aca="1" ref="B45" ca="1">TRANSPOSE(TRIM(MID(SUBSTITUTE(";"&amp;A45,";",REPT(" ",LEN(A45)+1)),ROW(INDIRECT("A1:A"&amp;LEN(A45)-LEN(SUBSTITUTE(A45,";",""))+1))*LEN(A45)+1,LEN(A45)+1)))</f>
         <v/>
@@ -2440,7 +2524,7 @@
       <c r="AB45" s="1"/>
       <c r="AC45" s="1"/>
     </row>
-    <row r="46" spans="2:29" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:29">
       <c r="B46" s="1" t="str" cm="1">
         <f t="array" aca="1" ref="B46" ca="1">TRANSPOSE(TRIM(MID(SUBSTITUTE(";"&amp;A46,";",REPT(" ",LEN(A46)+1)),ROW(INDIRECT("A1:A"&amp;LEN(A46)-LEN(SUBSTITUTE(A46,";",""))+1))*LEN(A46)+1,LEN(A46)+1)))</f>
         <v/>
@@ -2473,7 +2557,7 @@
       <c r="AB46" s="1"/>
       <c r="AC46" s="1"/>
     </row>
-    <row r="47" spans="2:29" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:29">
       <c r="B47" s="1" t="str" cm="1">
         <f t="array" aca="1" ref="B47" ca="1">TRANSPOSE(TRIM(MID(SUBSTITUTE(";"&amp;A47,";",REPT(" ",LEN(A47)+1)),ROW(INDIRECT("A1:A"&amp;LEN(A47)-LEN(SUBSTITUTE(A47,";",""))+1))*LEN(A47)+1,LEN(A47)+1)))</f>
         <v/>
@@ -2506,7 +2590,7 @@
       <c r="AB47" s="1"/>
       <c r="AC47" s="1"/>
     </row>
-    <row r="48" spans="2:29" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:29">
       <c r="B48" s="1" t="str" cm="1">
         <f t="array" aca="1" ref="B48" ca="1">TRANSPOSE(TRIM(MID(SUBSTITUTE(";"&amp;A48,";",REPT(" ",LEN(A48)+1)),ROW(INDIRECT("A1:A"&amp;LEN(A48)-LEN(SUBSTITUTE(A48,";",""))+1))*LEN(A48)+1,LEN(A48)+1)))</f>
         <v/>
@@ -2539,7 +2623,7 @@
       <c r="AB48" s="1"/>
       <c r="AC48" s="1"/>
     </row>
-    <row r="49" spans="2:29" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:29">
       <c r="B49" s="1" t="str" cm="1">
         <f t="array" aca="1" ref="B49" ca="1">TRANSPOSE(TRIM(MID(SUBSTITUTE(";"&amp;A49,";",REPT(" ",LEN(A49)+1)),ROW(INDIRECT("A1:A"&amp;LEN(A49)-LEN(SUBSTITUTE(A49,";",""))+1))*LEN(A49)+1,LEN(A49)+1)))</f>
         <v/>
@@ -2572,7 +2656,7 @@
       <c r="AB49" s="1"/>
       <c r="AC49" s="1"/>
     </row>
-    <row r="50" spans="2:29" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:29">
       <c r="B50" s="1" t="str" cm="1">
         <f t="array" aca="1" ref="B50" ca="1">TRANSPOSE(TRIM(MID(SUBSTITUTE(";"&amp;A50,";",REPT(" ",LEN(A50)+1)),ROW(INDIRECT("A1:A"&amp;LEN(A50)-LEN(SUBSTITUTE(A50,";",""))+1))*LEN(A50)+1,LEN(A50)+1)))</f>
         <v/>
@@ -2605,7 +2689,7 @@
       <c r="AB50" s="1"/>
       <c r="AC50" s="1"/>
     </row>
-    <row r="51" spans="2:29" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:29">
       <c r="B51" s="1" t="str" cm="1">
         <f t="array" aca="1" ref="B51" ca="1">TRANSPOSE(TRIM(MID(SUBSTITUTE(";"&amp;A51,";",REPT(" ",LEN(A51)+1)),ROW(INDIRECT("A1:A"&amp;LEN(A51)-LEN(SUBSTITUTE(A51,";",""))+1))*LEN(A51)+1,LEN(A51)+1)))</f>
         <v/>
@@ -2638,7 +2722,7 @@
       <c r="AB51" s="1"/>
       <c r="AC51" s="1"/>
     </row>
-    <row r="52" spans="2:29" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:29">
       <c r="B52" s="1" t="str" cm="1">
         <f t="array" aca="1" ref="B52" ca="1">TRANSPOSE(TRIM(MID(SUBSTITUTE(";"&amp;A52,";",REPT(" ",LEN(A52)+1)),ROW(INDIRECT("A1:A"&amp;LEN(A52)-LEN(SUBSTITUTE(A52,";",""))+1))*LEN(A52)+1,LEN(A52)+1)))</f>
         <v/>
@@ -2671,7 +2755,7 @@
       <c r="AB52" s="1"/>
       <c r="AC52" s="1"/>
     </row>
-    <row r="53" spans="2:29" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:29">
       <c r="B53" s="1" t="str" cm="1">
         <f t="array" aca="1" ref="B53" ca="1">TRANSPOSE(TRIM(MID(SUBSTITUTE(";"&amp;A53,";",REPT(" ",LEN(A53)+1)),ROW(INDIRECT("A1:A"&amp;LEN(A53)-LEN(SUBSTITUTE(A53,";",""))+1))*LEN(A53)+1,LEN(A53)+1)))</f>
         <v/>
@@ -2704,7 +2788,7 @@
       <c r="AB53" s="1"/>
       <c r="AC53" s="1"/>
     </row>
-    <row r="54" spans="2:29" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:29">
       <c r="B54" s="1" t="str" cm="1">
         <f t="array" aca="1" ref="B54" ca="1">TRANSPOSE(TRIM(MID(SUBSTITUTE(";"&amp;A54,";",REPT(" ",LEN(A54)+1)),ROW(INDIRECT("A1:A"&amp;LEN(A54)-LEN(SUBSTITUTE(A54,";",""))+1))*LEN(A54)+1,LEN(A54)+1)))</f>
         <v/>
@@ -2737,7 +2821,7 @@
       <c r="AB54" s="1"/>
       <c r="AC54" s="1"/>
     </row>
-    <row r="55" spans="2:29" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:29">
       <c r="B55" s="1" t="str" cm="1">
         <f t="array" aca="1" ref="B55" ca="1">TRANSPOSE(TRIM(MID(SUBSTITUTE(";"&amp;A55,";",REPT(" ",LEN(A55)+1)),ROW(INDIRECT("A1:A"&amp;LEN(A55)-LEN(SUBSTITUTE(A55,";",""))+1))*LEN(A55)+1,LEN(A55)+1)))</f>
         <v/>
@@ -2770,7 +2854,7 @@
       <c r="AB55" s="1"/>
       <c r="AC55" s="1"/>
     </row>
-    <row r="56" spans="2:29" x14ac:dyDescent="0.2">
+    <row r="56" spans="2:29">
       <c r="B56" s="1" t="str" cm="1">
         <f t="array" aca="1" ref="B56" ca="1">TRANSPOSE(TRIM(MID(SUBSTITUTE(";"&amp;A56,";",REPT(" ",LEN(A56)+1)),ROW(INDIRECT("A1:A"&amp;LEN(A56)-LEN(SUBSTITUTE(A56,";",""))+1))*LEN(A56)+1,LEN(A56)+1)))</f>
         <v/>
@@ -2803,7 +2887,7 @@
       <c r="AB56" s="1"/>
       <c r="AC56" s="1"/>
     </row>
-    <row r="57" spans="2:29" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:29">
       <c r="B57" s="1" t="str" cm="1">
         <f t="array" aca="1" ref="B57" ca="1">TRANSPOSE(TRIM(MID(SUBSTITUTE(";"&amp;A57,";",REPT(" ",LEN(A57)+1)),ROW(INDIRECT("A1:A"&amp;LEN(A57)-LEN(SUBSTITUTE(A57,";",""))+1))*LEN(A57)+1,LEN(A57)+1)))</f>
         <v/>
@@ -2836,7 +2920,7 @@
       <c r="AB57" s="1"/>
       <c r="AC57" s="1"/>
     </row>
-    <row r="58" spans="2:29" x14ac:dyDescent="0.2">
+    <row r="58" spans="2:29">
       <c r="B58" s="1" t="str" cm="1">
         <f t="array" aca="1" ref="B58" ca="1">TRANSPOSE(TRIM(MID(SUBSTITUTE(";"&amp;A58,";",REPT(" ",LEN(A58)+1)),ROW(INDIRECT("A1:A"&amp;LEN(A58)-LEN(SUBSTITUTE(A58,";",""))+1))*LEN(A58)+1,LEN(A58)+1)))</f>
         <v/>
@@ -2869,7 +2953,7 @@
       <c r="AB58" s="1"/>
       <c r="AC58" s="1"/>
     </row>
-    <row r="59" spans="2:29" x14ac:dyDescent="0.2">
+    <row r="59" spans="2:29">
       <c r="B59" s="1" t="str" cm="1">
         <f t="array" aca="1" ref="B59" ca="1">TRANSPOSE(TRIM(MID(SUBSTITUTE(";"&amp;A59,";",REPT(" ",LEN(A59)+1)),ROW(INDIRECT("A1:A"&amp;LEN(A59)-LEN(SUBSTITUTE(A59,";",""))+1))*LEN(A59)+1,LEN(A59)+1)))</f>
         <v/>
@@ -2902,7 +2986,7 @@
       <c r="AB59" s="1"/>
       <c r="AC59" s="1"/>
     </row>
-    <row r="60" spans="2:29" x14ac:dyDescent="0.2">
+    <row r="60" spans="2:29">
       <c r="B60" s="1" t="str" cm="1">
         <f t="array" aca="1" ref="B60" ca="1">TRANSPOSE(TRIM(MID(SUBSTITUTE(";"&amp;A60,";",REPT(" ",LEN(A60)+1)),ROW(INDIRECT("A1:A"&amp;LEN(A60)-LEN(SUBSTITUTE(A60,";",""))+1))*LEN(A60)+1,LEN(A60)+1)))</f>
         <v/>
@@ -2935,7 +3019,7 @@
       <c r="AB60" s="1"/>
       <c r="AC60" s="1"/>
     </row>
-    <row r="61" spans="2:29" x14ac:dyDescent="0.2">
+    <row r="61" spans="2:29">
       <c r="B61" s="1" t="str" cm="1">
         <f t="array" aca="1" ref="B61" ca="1">TRANSPOSE(TRIM(MID(SUBSTITUTE(";"&amp;A61,";",REPT(" ",LEN(A61)+1)),ROW(INDIRECT("A1:A"&amp;LEN(A61)-LEN(SUBSTITUTE(A61,";",""))+1))*LEN(A61)+1,LEN(A61)+1)))</f>
         <v/>
@@ -2968,7 +3052,7 @@
       <c r="AB61" s="1"/>
       <c r="AC61" s="1"/>
     </row>
-    <row r="62" spans="2:29" x14ac:dyDescent="0.2">
+    <row r="62" spans="2:29">
       <c r="B62" s="1" t="str" cm="1">
         <f t="array" aca="1" ref="B62" ca="1">TRANSPOSE(TRIM(MID(SUBSTITUTE(";"&amp;A62,";",REPT(" ",LEN(A62)+1)),ROW(INDIRECT("A1:A"&amp;LEN(A62)-LEN(SUBSTITUTE(A62,";",""))+1))*LEN(A62)+1,LEN(A62)+1)))</f>
         <v/>
@@ -3001,7 +3085,7 @@
       <c r="AB62" s="1"/>
       <c r="AC62" s="1"/>
     </row>
-    <row r="63" spans="2:29" x14ac:dyDescent="0.2">
+    <row r="63" spans="2:29">
       <c r="B63" s="1" t="str" cm="1">
         <f t="array" aca="1" ref="B63" ca="1">TRANSPOSE(TRIM(MID(SUBSTITUTE(";"&amp;A63,";",REPT(" ",LEN(A63)+1)),ROW(INDIRECT("A1:A"&amp;LEN(A63)-LEN(SUBSTITUTE(A63,";",""))+1))*LEN(A63)+1,LEN(A63)+1)))</f>
         <v/>
@@ -3034,7 +3118,7 @@
       <c r="AB63" s="1"/>
       <c r="AC63" s="1"/>
     </row>
-    <row r="64" spans="2:29" x14ac:dyDescent="0.2">
+    <row r="64" spans="2:29">
       <c r="B64" s="1" t="str" cm="1">
         <f t="array" aca="1" ref="B64" ca="1">TRANSPOSE(TRIM(MID(SUBSTITUTE(";"&amp;A64,";",REPT(" ",LEN(A64)+1)),ROW(INDIRECT("A1:A"&amp;LEN(A64)-LEN(SUBSTITUTE(A64,";",""))+1))*LEN(A64)+1,LEN(A64)+1)))</f>
         <v/>
@@ -3067,7 +3151,7 @@
       <c r="AB64" s="1"/>
       <c r="AC64" s="1"/>
     </row>
-    <row r="65" spans="2:29" x14ac:dyDescent="0.2">
+    <row r="65" spans="2:29">
       <c r="B65" s="1" t="str" cm="1">
         <f t="array" aca="1" ref="B65" ca="1">TRANSPOSE(TRIM(MID(SUBSTITUTE(";"&amp;A65,";",REPT(" ",LEN(A65)+1)),ROW(INDIRECT("A1:A"&amp;LEN(A65)-LEN(SUBSTITUTE(A65,";",""))+1))*LEN(A65)+1,LEN(A65)+1)))</f>
         <v/>
@@ -3100,7 +3184,7 @@
       <c r="AB65" s="1"/>
       <c r="AC65" s="1"/>
     </row>
-    <row r="66" spans="2:29" x14ac:dyDescent="0.2">
+    <row r="66" spans="2:29">
       <c r="B66" s="1" t="str" cm="1">
         <f t="array" aca="1" ref="B66" ca="1">TRANSPOSE(TRIM(MID(SUBSTITUTE(";"&amp;A66,";",REPT(" ",LEN(A66)+1)),ROW(INDIRECT("A1:A"&amp;LEN(A66)-LEN(SUBSTITUTE(A66,";",""))+1))*LEN(A66)+1,LEN(A66)+1)))</f>
         <v/>
@@ -3133,7 +3217,7 @@
       <c r="AB66" s="1"/>
       <c r="AC66" s="1"/>
     </row>
-    <row r="67" spans="2:29" x14ac:dyDescent="0.2">
+    <row r="67" spans="2:29">
       <c r="B67" s="1" t="str" cm="1">
         <f t="array" aca="1" ref="B67" ca="1">TRANSPOSE(TRIM(MID(SUBSTITUTE(";"&amp;A67,";",REPT(" ",LEN(A67)+1)),ROW(INDIRECT("A1:A"&amp;LEN(A67)-LEN(SUBSTITUTE(A67,";",""))+1))*LEN(A67)+1,LEN(A67)+1)))</f>
         <v/>
@@ -3166,7 +3250,7 @@
       <c r="AB67" s="1"/>
       <c r="AC67" s="1"/>
     </row>
-    <row r="68" spans="2:29" x14ac:dyDescent="0.2">
+    <row r="68" spans="2:29">
       <c r="B68" s="1" t="str" cm="1">
         <f t="array" aca="1" ref="B68" ca="1">TRANSPOSE(TRIM(MID(SUBSTITUTE(";"&amp;A68,";",REPT(" ",LEN(A68)+1)),ROW(INDIRECT("A1:A"&amp;LEN(A68)-LEN(SUBSTITUTE(A68,";",""))+1))*LEN(A68)+1,LEN(A68)+1)))</f>
         <v/>
@@ -3199,7 +3283,7 @@
       <c r="AB68" s="1"/>
       <c r="AC68" s="1"/>
     </row>
-    <row r="69" spans="2:29" x14ac:dyDescent="0.2">
+    <row r="69" spans="2:29">
       <c r="B69" s="1" t="str" cm="1">
         <f t="array" aca="1" ref="B69" ca="1">TRANSPOSE(TRIM(MID(SUBSTITUTE(";"&amp;A69,";",REPT(" ",LEN(A69)+1)),ROW(INDIRECT("A1:A"&amp;LEN(A69)-LEN(SUBSTITUTE(A69,";",""))+1))*LEN(A69)+1,LEN(A69)+1)))</f>
         <v/>
@@ -3232,7 +3316,7 @@
       <c r="AB69" s="1"/>
       <c r="AC69" s="1"/>
     </row>
-    <row r="70" spans="2:29" x14ac:dyDescent="0.2">
+    <row r="70" spans="2:29">
       <c r="B70" s="1" t="str" cm="1">
         <f t="array" aca="1" ref="B70" ca="1">TRANSPOSE(TRIM(MID(SUBSTITUTE(";"&amp;A70,";",REPT(" ",LEN(A70)+1)),ROW(INDIRECT("A1:A"&amp;LEN(A70)-LEN(SUBSTITUTE(A70,";",""))+1))*LEN(A70)+1,LEN(A70)+1)))</f>
         <v/>
@@ -3280,13 +3364,13 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="20.6640625" customWidth="1"/>
-    <col min="2" max="29" width="10.6640625" customWidth="1"/>
+    <col min="1" max="1" width="20.7109375" customWidth="1"/>
+    <col min="2" max="29" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:42">
       <c r="A1">
         <f>Insert!A1</f>
         <v>0</v>
@@ -3387,7 +3471,7 @@
       <c r="AO1" s="3"/>
       <c r="AP1" s="3"/>
     </row>
-    <row r="2" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:42">
       <c r="A2" t="str">
         <f>Insert!A2</f>
         <v>s=Name Surname;e=2022 Izmir Regional;l=f;m=1;r=r1;t=6838;as=[42];at=Y;au=3;al=2;ac=Y;tu=4;tl=2;tm=1;tn=2;wd=Y;cl=t;ss=[19,11,33,21,71,56];c=3;be=Y;cn=2;ds=v;dr=v;d=N;to=N;cf=Y;co=Abi Gerçekten Çok güzel olmuş site</v>
@@ -3515,7 +3599,7 @@
       <c r="AO2" s="4"/>
       <c r="AP2" s="4"/>
     </row>
-    <row r="3" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:42">
       <c r="A3">
         <f>Insert!A3</f>
         <v>0</v>
@@ -3567,41 +3651,119 @@
       <c r="AO3" s="4"/>
       <c r="AP3" s="4"/>
     </row>
-    <row r="4" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="A4">
+    <row r="4" spans="1:42">
+      <c r="A4" t="str">
         <f>Insert!A4</f>
-        <v>0</v>
-      </c>
-      <c r="B4" s="1" t="e" cm="1">
-        <f t="array" aca="1" ref="B4" ca="1">RIGHT(_xlfn.ANCHORARRAY(Insert!B4), LEN(_xlfn.ANCHORARRAY(Insert!B4)) - FIND("=",_xlfn.ANCHORARRAY( Insert!B4)))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
-      <c r="L4" s="1"/>
-      <c r="M4" s="1"/>
-      <c r="N4" s="1"/>
-      <c r="O4" s="1"/>
-      <c r="P4" s="1"/>
-      <c r="Q4" s="1"/>
-      <c r="R4" s="1"/>
-      <c r="S4" s="1"/>
-      <c r="T4" s="1"/>
-      <c r="U4" s="1"/>
-      <c r="V4" s="1"/>
-      <c r="W4" s="1"/>
-      <c r="X4" s="1"/>
-      <c r="Y4" s="1"/>
-      <c r="Z4" s="1"/>
-      <c r="AA4" s="1"/>
-      <c r="AB4" s="1"/>
+        <v>s=Yiğit Emre Çulcuoğlu;e=2022 İzmir Regional;l=f;m=1;r=b2;t=6838;as=[54];at=Y;au=8;al=3;ac=Y;tu=5;tl=6;tm=1;tn=2;wd=Y;cl=b;ss=[53,56,44,58,34,20,17,18,41,51,51,16,26,50,64,68,34];c=4;be=Y;cn=1;ds=v;dr=v;d=N;to=N;cf=N;co=Commen</v>
+      </c>
+      <c r="B4" s="1" t="str" cm="1">
+        <f t="array" aca="1" ref="B4:AB4" ca="1">RIGHT(_xlfn.ANCHORARRAY(Insert!B4), LEN(_xlfn.ANCHORARRAY(Insert!B4)) - FIND("=",_xlfn.ANCHORARRAY( Insert!B4)))</f>
+        <v>Yiğit Emre Çulcuoğlu</v>
+      </c>
+      <c r="C4" s="1" t="str">
+        <f ca="1"/>
+        <v>2022 İzmir Regional</v>
+      </c>
+      <c r="D4" s="1" t="str">
+        <f ca="1"/>
+        <v>f</v>
+      </c>
+      <c r="E4" s="1" t="str">
+        <f ca="1"/>
+        <v>1</v>
+      </c>
+      <c r="F4" s="1" t="str">
+        <f ca="1"/>
+        <v>b2</v>
+      </c>
+      <c r="G4" s="1" t="str">
+        <f ca="1"/>
+        <v>6838</v>
+      </c>
+      <c r="H4" s="1" t="str">
+        <f ca="1"/>
+        <v>[54]</v>
+      </c>
+      <c r="I4" s="1" t="str">
+        <f ca="1"/>
+        <v>Y</v>
+      </c>
+      <c r="J4" s="1" t="str">
+        <f ca="1"/>
+        <v>8</v>
+      </c>
+      <c r="K4" s="1" t="str">
+        <f ca="1"/>
+        <v>3</v>
+      </c>
+      <c r="L4" s="1" t="str">
+        <f ca="1"/>
+        <v>Y</v>
+      </c>
+      <c r="M4" s="1" t="str">
+        <f ca="1"/>
+        <v>5</v>
+      </c>
+      <c r="N4" s="1" t="str">
+        <f ca="1"/>
+        <v>6</v>
+      </c>
+      <c r="O4" s="1" t="str">
+        <f ca="1"/>
+        <v>1</v>
+      </c>
+      <c r="P4" s="1" t="str">
+        <f ca="1"/>
+        <v>2</v>
+      </c>
+      <c r="Q4" s="1" t="str">
+        <f ca="1"/>
+        <v>Y</v>
+      </c>
+      <c r="R4" s="1" t="str">
+        <f ca="1"/>
+        <v>b</v>
+      </c>
+      <c r="S4" s="1" t="str">
+        <f ca="1"/>
+        <v>[53,56,44,58,34,20,17,18,41,51,51,16,26,50,64,68,34]</v>
+      </c>
+      <c r="T4" s="1" t="str">
+        <f ca="1"/>
+        <v>4</v>
+      </c>
+      <c r="U4" s="1" t="str">
+        <f ca="1"/>
+        <v>Y</v>
+      </c>
+      <c r="V4" s="1" t="str">
+        <f ca="1"/>
+        <v>1</v>
+      </c>
+      <c r="W4" s="1" t="str">
+        <f ca="1"/>
+        <v>v</v>
+      </c>
+      <c r="X4" s="1" t="str">
+        <f ca="1"/>
+        <v>v</v>
+      </c>
+      <c r="Y4" s="1" t="str">
+        <f ca="1"/>
+        <v>N</v>
+      </c>
+      <c r="Z4" s="1" t="str">
+        <f ca="1"/>
+        <v>N</v>
+      </c>
+      <c r="AA4" s="1" t="str">
+        <f ca="1"/>
+        <v>N</v>
+      </c>
+      <c r="AB4" s="1" t="str">
+        <f ca="1"/>
+        <v>Commen</v>
+      </c>
       <c r="AC4" s="1"/>
       <c r="AD4" s="4"/>
       <c r="AE4" s="4"/>
@@ -3617,7 +3779,7 @@
       <c r="AO4" s="4"/>
       <c r="AP4" s="4"/>
     </row>
-    <row r="5" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:42">
       <c r="A5">
         <f>Insert!A5</f>
         <v>0</v>
@@ -3667,7 +3829,7 @@
       <c r="AO5" s="4"/>
       <c r="AP5" s="4"/>
     </row>
-    <row r="6" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:42">
       <c r="A6">
         <f>Insert!A6</f>
         <v>0</v>
@@ -3717,7 +3879,7 @@
       <c r="AO6" s="4"/>
       <c r="AP6" s="4"/>
     </row>
-    <row r="7" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:42">
       <c r="A7">
         <f>Insert!A7</f>
         <v>0</v>
@@ -3767,7 +3929,7 @@
       <c r="AO7" s="4"/>
       <c r="AP7" s="4"/>
     </row>
-    <row r="8" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:42">
       <c r="A8">
         <f>Insert!A8</f>
         <v>0</v>
@@ -3817,7 +3979,7 @@
       <c r="AO8" s="4"/>
       <c r="AP8" s="4"/>
     </row>
-    <row r="9" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:42">
       <c r="A9">
         <f>Insert!A9</f>
         <v>0</v>
@@ -3867,7 +4029,7 @@
       <c r="AO9" s="4"/>
       <c r="AP9" s="4"/>
     </row>
-    <row r="10" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:42">
       <c r="A10">
         <f>Insert!A10</f>
         <v>0</v>
@@ -3917,7 +4079,7 @@
       <c r="AO10" s="4"/>
       <c r="AP10" s="4"/>
     </row>
-    <row r="11" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:42">
       <c r="A11">
         <f>Insert!A11</f>
         <v>0</v>
@@ -3967,7 +4129,7 @@
       <c r="AO11" s="4"/>
       <c r="AP11" s="4"/>
     </row>
-    <row r="12" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:42">
       <c r="A12">
         <f>Insert!A12</f>
         <v>0</v>
@@ -4017,7 +4179,7 @@
       <c r="AO12" s="4"/>
       <c r="AP12" s="4"/>
     </row>
-    <row r="13" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:42">
       <c r="A13">
         <f>Insert!A13</f>
         <v>0</v>
@@ -4067,7 +4229,7 @@
       <c r="AO13" s="4"/>
       <c r="AP13" s="4"/>
     </row>
-    <row r="14" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:42">
       <c r="A14">
         <f>Insert!A14</f>
         <v>0</v>
@@ -4117,7 +4279,7 @@
       <c r="AO14" s="4"/>
       <c r="AP14" s="4"/>
     </row>
-    <row r="15" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:42">
       <c r="A15">
         <f>Insert!A15</f>
         <v>0</v>
@@ -4167,7 +4329,7 @@
       <c r="AO15" s="4"/>
       <c r="AP15" s="4"/>
     </row>
-    <row r="16" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:42">
       <c r="A16">
         <f>Insert!A16</f>
         <v>0</v>
@@ -4217,7 +4379,7 @@
       <c r="AO16" s="4"/>
       <c r="AP16" s="4"/>
     </row>
-    <row r="17" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:42">
       <c r="A17">
         <f>Insert!A17</f>
         <v>0</v>
@@ -4267,7 +4429,7 @@
       <c r="AO17" s="4"/>
       <c r="AP17" s="4"/>
     </row>
-    <row r="18" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:42">
       <c r="A18">
         <f>Insert!A18</f>
         <v>0</v>
@@ -4317,7 +4479,7 @@
       <c r="AO18" s="4"/>
       <c r="AP18" s="4"/>
     </row>
-    <row r="19" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:42">
       <c r="A19">
         <f>Insert!A19</f>
         <v>0</v>

</xml_diff>

<commit_message>
Practice match option is added for match level + Team Name section
</commit_message>
<xml_diff>
--- a/Excel/Excel.xlsx
+++ b/Excel/Excel.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yigit\Desktop\ScoutingApp6838\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\github\6838scout\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9821CF57-702F-4D62-B17E-93941376B362}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8326B072-6C9E-41B2-ABFA-6573167CAC11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A46E49DD-D669-429F-AA31-B068C359770D}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="29">
   <si>
     <t>Scouter</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -81,9 +81,6 @@
   <si>
     <t>Was Defended</t>
     <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>s=Name Surname;e=2022 Izmir Regional;l=f;m=1;r=r1;t=6838;as=[42];at=Y;au=3;al=2;ac=Y;tu=4;tl=2;tm=1;tn=2;wd=Y;cl=t;ss=[19,11,33,21,71,56];c=3;be=Y;cn=2;ds=v;dr=v;d=N;to=N;cf=Y;co=Abi Gerçekten Çok güzel olmuş site</t>
   </si>
   <si>
     <t>M Upper Cargo Scored</t>
@@ -152,7 +149,7 @@
     <t>Team</t>
   </si>
   <si>
-    <t>s=Yiğit Emre Çulcuoğlu;e=2022 İzmir Regional;l=f;m=1;r=b2;t=6838;as=[54];at=Y;au=8;al=3;ac=Y;tu=5;tl=6;tm=1;tn=2;wd=Y;cl=b;ss=[53,56,44,58,34,20,17,18,41,51,51,16,26,50,64,68,34];c=4;be=Y;cn=1;ds=v;dr=v;d=N;to=N;cf=N;co=Commen</t>
+    <t>Team Name</t>
   </si>
 </sst>
 </file>
@@ -593,7 +590,7 @@
   <dimension ref="A1:AP70"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -610,7 +607,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>2</v>
@@ -619,28 +616,28 @@
         <v>3</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="L1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>7</v>
-      </c>
       <c r="N1" s="2" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="O1" s="2" t="s">
         <v>9</v>
@@ -649,43 +646,45 @@
         <v>8</v>
       </c>
       <c r="Q1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="R1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="S1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="T1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="U1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="V1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="W1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="X1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="Y1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="Z1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="Y1" s="2" t="s">
+      <c r="AA1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="AB1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="AA1" s="2" t="s">
+      <c r="AC1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="AB1" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="AC1" s="5"/>
-      <c r="AD1" s="3"/>
+      <c r="AD1" s="5"/>
       <c r="AE1" s="3"/>
       <c r="AF1" s="3"/>
       <c r="AG1" s="3"/>
@@ -693,119 +692,40 @@
       <c r="AI1" s="3"/>
       <c r="AJ1" s="3"/>
       <c r="AK1" s="3"/>
+      <c r="AL1" s="3"/>
     </row>
     <row r="2" spans="1:42" ht="20.25">
-      <c r="A2" s="6" t="s">
-        <v>6</v>
-      </c>
+      <c r="A2" s="6"/>
       <c r="B2" s="1" t="str" cm="1">
-        <f t="array" aca="1" ref="B2:AB2" ca="1">TRANSPOSE(TRIM(MID(SUBSTITUTE(";"&amp;A2,";",REPT(" ",LEN(A2)+1)),ROW(INDIRECT("A1:A"&amp;LEN(A2)-LEN(SUBSTITUTE(A2,";",""))+1))*LEN(A2)+1,LEN(A2)+1)))</f>
-        <v>s=Name Surname</v>
-      </c>
-      <c r="C2" s="1" t="str">
-        <f ca="1"/>
-        <v>e=2022 Izmir Regional</v>
-      </c>
-      <c r="D2" s="1" t="str">
-        <f ca="1"/>
-        <v>l=f</v>
-      </c>
-      <c r="E2" s="1" t="str">
-        <f ca="1"/>
-        <v>m=1</v>
-      </c>
-      <c r="F2" s="1" t="str">
-        <f ca="1"/>
-        <v>r=r1</v>
-      </c>
-      <c r="G2" s="1" t="str">
-        <f ca="1"/>
-        <v>t=6838</v>
-      </c>
-      <c r="H2" s="1" t="str">
-        <f ca="1"/>
-        <v>as=[42]</v>
-      </c>
-      <c r="I2" s="1" t="str">
-        <f ca="1"/>
-        <v>at=Y</v>
-      </c>
-      <c r="J2" s="1" t="str">
-        <f ca="1"/>
-        <v>au=3</v>
-      </c>
-      <c r="K2" s="1" t="str">
-        <f ca="1"/>
-        <v>al=2</v>
-      </c>
-      <c r="L2" s="1" t="str">
-        <f ca="1"/>
-        <v>ac=Y</v>
-      </c>
-      <c r="M2" s="1" t="str">
-        <f ca="1"/>
-        <v>tu=4</v>
-      </c>
-      <c r="N2" s="1" t="str">
-        <f ca="1"/>
-        <v>tl=2</v>
-      </c>
-      <c r="O2" s="1" t="str">
-        <f ca="1"/>
-        <v>tm=1</v>
-      </c>
-      <c r="P2" s="1" t="str">
-        <f ca="1"/>
-        <v>tn=2</v>
-      </c>
-      <c r="Q2" s="1" t="str">
-        <f ca="1"/>
-        <v>wd=Y</v>
-      </c>
-      <c r="R2" s="1" t="str">
-        <f ca="1"/>
-        <v>cl=t</v>
-      </c>
-      <c r="S2" s="1" t="str">
-        <f ca="1"/>
-        <v>ss=[19,11,33,21,71,56]</v>
-      </c>
-      <c r="T2" s="1" t="str">
-        <f ca="1"/>
-        <v>c=3</v>
-      </c>
-      <c r="U2" s="1" t="str">
-        <f ca="1"/>
-        <v>be=Y</v>
-      </c>
-      <c r="V2" s="1" t="str">
-        <f ca="1"/>
-        <v>cn=2</v>
-      </c>
-      <c r="W2" s="1" t="str">
-        <f ca="1"/>
-        <v>ds=v</v>
-      </c>
-      <c r="X2" s="1" t="str">
-        <f ca="1"/>
-        <v>dr=v</v>
-      </c>
-      <c r="Y2" s="1" t="str">
-        <f ca="1"/>
-        <v>d=N</v>
-      </c>
-      <c r="Z2" s="1" t="str">
-        <f ca="1"/>
-        <v>to=N</v>
-      </c>
-      <c r="AA2" s="1" t="str">
-        <f ca="1"/>
-        <v>cf=Y</v>
-      </c>
-      <c r="AB2" s="1" t="str">
-        <f ca="1"/>
-        <v>co=Abi Gerçekten Çok güzel olmuş site</v>
-      </c>
+        <f t="array" aca="1" ref="B2" ca="1">TRANSPOSE(TRIM(MID(SUBSTITUTE(";"&amp;A2,";",REPT(" ",LEN(A2)+1)),ROW(INDIRECT("A1:A"&amp;LEN(A2)-LEN(SUBSTITUTE(A2,";",""))+1))*LEN(A2)+1,LEN(A2)+1)))</f>
+        <v/>
+      </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
+      <c r="R2" s="1"/>
+      <c r="S2" s="1"/>
+      <c r="T2" s="1"/>
+      <c r="U2" s="1"/>
+      <c r="V2" s="1"/>
+      <c r="W2" s="1"/>
+      <c r="X2" s="1"/>
+      <c r="Y2" s="1"/>
+      <c r="Z2" s="1"/>
+      <c r="AA2" s="1"/>
+      <c r="AB2" s="1"/>
       <c r="AC2" s="1"/>
       <c r="AD2" s="4"/>
       <c r="AE2" s="4"/>
@@ -866,117 +786,36 @@
       <c r="AP3" s="4"/>
     </row>
     <row r="4" spans="1:42">
-      <c r="A4" t="s">
-        <v>29</v>
-      </c>
       <c r="B4" s="1" t="str" cm="1">
-        <f t="array" aca="1" ref="B4:AB4" ca="1">TRANSPOSE(TRIM(MID(SUBSTITUTE(";"&amp;A4,";",REPT(" ",LEN(A4)+1)),ROW(INDIRECT("A1:A"&amp;LEN(A4)-LEN(SUBSTITUTE(A4,";",""))+1))*LEN(A4)+1,LEN(A4)+1)))</f>
-        <v>s=Yiğit Emre Çulcuoğlu</v>
-      </c>
-      <c r="C4" s="1" t="str">
-        <f ca="1"/>
-        <v>e=2022 İzmir Regional</v>
-      </c>
-      <c r="D4" s="1" t="str">
-        <f ca="1"/>
-        <v>l=f</v>
-      </c>
-      <c r="E4" s="1" t="str">
-        <f ca="1"/>
-        <v>m=1</v>
-      </c>
-      <c r="F4" s="1" t="str">
-        <f ca="1"/>
-        <v>r=b2</v>
-      </c>
-      <c r="G4" s="1" t="str">
-        <f ca="1"/>
-        <v>t=6838</v>
-      </c>
-      <c r="H4" s="1" t="str">
-        <f ca="1"/>
-        <v>as=[54]</v>
-      </c>
-      <c r="I4" s="1" t="str">
-        <f ca="1"/>
-        <v>at=Y</v>
-      </c>
-      <c r="J4" s="1" t="str">
-        <f ca="1"/>
-        <v>au=8</v>
-      </c>
-      <c r="K4" s="1" t="str">
-        <f ca="1"/>
-        <v>al=3</v>
-      </c>
-      <c r="L4" s="1" t="str">
-        <f ca="1"/>
-        <v>ac=Y</v>
-      </c>
-      <c r="M4" s="1" t="str">
-        <f ca="1"/>
-        <v>tu=5</v>
-      </c>
-      <c r="N4" s="1" t="str">
-        <f ca="1"/>
-        <v>tl=6</v>
-      </c>
-      <c r="O4" s="1" t="str">
-        <f ca="1"/>
-        <v>tm=1</v>
-      </c>
-      <c r="P4" s="1" t="str">
-        <f ca="1"/>
-        <v>tn=2</v>
-      </c>
-      <c r="Q4" s="1" t="str">
-        <f ca="1"/>
-        <v>wd=Y</v>
-      </c>
-      <c r="R4" s="1" t="str">
-        <f ca="1"/>
-        <v>cl=b</v>
-      </c>
-      <c r="S4" s="1" t="str">
-        <f ca="1"/>
-        <v>ss=[53,56,44,58,34,20,17,18,41,51,51,16,26,50,64,68,34]</v>
-      </c>
-      <c r="T4" s="1" t="str">
-        <f ca="1"/>
-        <v>c=4</v>
-      </c>
-      <c r="U4" s="1" t="str">
-        <f ca="1"/>
-        <v>be=Y</v>
-      </c>
-      <c r="V4" s="1" t="str">
-        <f ca="1"/>
-        <v>cn=1</v>
-      </c>
-      <c r="W4" s="1" t="str">
-        <f ca="1"/>
-        <v>ds=v</v>
-      </c>
-      <c r="X4" s="1" t="str">
-        <f ca="1"/>
-        <v>dr=v</v>
-      </c>
-      <c r="Y4" s="1" t="str">
-        <f ca="1"/>
-        <v>d=N</v>
-      </c>
-      <c r="Z4" s="1" t="str">
-        <f ca="1"/>
-        <v>to=N</v>
-      </c>
-      <c r="AA4" s="1" t="str">
-        <f ca="1"/>
-        <v>cf=N</v>
-      </c>
-      <c r="AB4" s="1" t="str">
-        <f ca="1"/>
-        <v>co=Commen</v>
-      </c>
+        <f t="array" aca="1" ref="B4" ca="1">TRANSPOSE(TRIM(MID(SUBSTITUTE(";"&amp;A4,";",REPT(" ",LEN(A4)+1)),ROW(INDIRECT("A1:A"&amp;LEN(A4)-LEN(SUBSTITUTE(A4,";",""))+1))*LEN(A4)+1,LEN(A4)+1)))</f>
+        <v/>
+      </c>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
+      <c r="Q4" s="1"/>
+      <c r="R4" s="1"/>
+      <c r="S4" s="1"/>
+      <c r="T4" s="1"/>
+      <c r="U4" s="1"/>
+      <c r="V4" s="1"/>
+      <c r="W4" s="1"/>
+      <c r="X4" s="1"/>
+      <c r="Y4" s="1"/>
+      <c r="Z4" s="1"/>
+      <c r="AA4" s="1"/>
+      <c r="AB4" s="1"/>
       <c r="AC4" s="1"/>
       <c r="AD4" s="4"/>
       <c r="AE4" s="4"/>
@@ -3358,10 +3197,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1048276-8A82-4E9E-96B8-21ABC897CB97}">
-  <dimension ref="A1:AP19"/>
+  <dimension ref="A1:AQ19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -3370,7 +3209,7 @@
     <col min="2" max="29" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:42">
+    <row r="1" spans="1:43">
       <c r="A1">
         <f>Insert!A1</f>
         <v>0</v>
@@ -3382,7 +3221,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>2</v>
@@ -3391,28 +3230,28 @@
         <v>3</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="L1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>7</v>
-      </c>
       <c r="N1" s="2" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="O1" s="2" t="s">
         <v>9</v>
@@ -3421,43 +3260,45 @@
         <v>8</v>
       </c>
       <c r="Q1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="R1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="S1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="T1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="U1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="V1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="W1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="X1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="Y1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="Z1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="Y1" s="2" t="s">
+      <c r="AA1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="AB1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="AA1" s="2" t="s">
+      <c r="AC1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="AB1" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="AC1" s="5"/>
-      <c r="AD1" s="3"/>
+      <c r="AD1" s="5"/>
       <c r="AE1" s="3"/>
       <c r="AF1" s="3"/>
       <c r="AG1" s="3"/>
@@ -3470,120 +3311,43 @@
       <c r="AN1" s="3"/>
       <c r="AO1" s="3"/>
       <c r="AP1" s="3"/>
-    </row>
-    <row r="2" spans="1:42">
-      <c r="A2" t="str">
+      <c r="AQ1" s="3"/>
+    </row>
+    <row r="2" spans="1:43">
+      <c r="A2">
         <f>Insert!A2</f>
-        <v>s=Name Surname;e=2022 Izmir Regional;l=f;m=1;r=r1;t=6838;as=[42];at=Y;au=3;al=2;ac=Y;tu=4;tl=2;tm=1;tn=2;wd=Y;cl=t;ss=[19,11,33,21,71,56];c=3;be=Y;cn=2;ds=v;dr=v;d=N;to=N;cf=Y;co=Abi Gerçekten Çok güzel olmuş site</v>
-      </c>
-      <c r="B2" s="1" t="str" cm="1">
-        <f t="array" aca="1" ref="B2:AB2" ca="1">RIGHT(_xlfn.ANCHORARRAY(Insert!B2), LEN(_xlfn.ANCHORARRAY(Insert!B2)) - FIND("=",_xlfn.ANCHORARRAY( Insert!B2)))</f>
-        <v>Name Surname</v>
-      </c>
-      <c r="C2" s="1" t="str">
-        <f ca="1"/>
-        <v>2022 Izmir Regional</v>
-      </c>
-      <c r="D2" s="1" t="str">
-        <f ca="1"/>
-        <v>f</v>
-      </c>
-      <c r="E2" s="1" t="str">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="F2" s="1" t="str">
-        <f ca="1"/>
-        <v>r1</v>
-      </c>
-      <c r="G2" s="1" t="str">
-        <f ca="1"/>
-        <v>6838</v>
-      </c>
-      <c r="H2" s="1" t="str">
-        <f ca="1"/>
-        <v>[42]</v>
-      </c>
-      <c r="I2" s="1" t="str">
-        <f ca="1"/>
-        <v>Y</v>
-      </c>
-      <c r="J2" s="1" t="str">
-        <f ca="1"/>
-        <v>3</v>
-      </c>
-      <c r="K2" s="1" t="str">
-        <f ca="1"/>
-        <v>2</v>
-      </c>
-      <c r="L2" s="1" t="str">
-        <f ca="1"/>
-        <v>Y</v>
-      </c>
-      <c r="M2" s="1" t="str">
-        <f ca="1"/>
-        <v>4</v>
-      </c>
-      <c r="N2" s="1" t="str">
-        <f ca="1"/>
-        <v>2</v>
-      </c>
-      <c r="O2" s="1" t="str">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="P2" s="1" t="str">
-        <f ca="1"/>
-        <v>2</v>
-      </c>
-      <c r="Q2" s="1" t="str">
-        <f ca="1"/>
-        <v>Y</v>
-      </c>
-      <c r="R2" s="1" t="str">
-        <f ca="1"/>
-        <v>t</v>
-      </c>
-      <c r="S2" s="1" t="str">
-        <f ca="1"/>
-        <v>[19,11,33,21,71,56]</v>
-      </c>
-      <c r="T2" s="1" t="str">
-        <f ca="1"/>
-        <v>3</v>
-      </c>
-      <c r="U2" s="1" t="str">
-        <f ca="1"/>
-        <v>Y</v>
-      </c>
-      <c r="V2" s="1" t="str">
-        <f ca="1"/>
-        <v>2</v>
-      </c>
-      <c r="W2" s="1" t="str">
-        <f ca="1"/>
-        <v>v</v>
-      </c>
-      <c r="X2" s="1" t="str">
-        <f ca="1"/>
-        <v>v</v>
-      </c>
-      <c r="Y2" s="1" t="str">
-        <f ca="1"/>
-        <v>N</v>
-      </c>
-      <c r="Z2" s="1" t="str">
-        <f ca="1"/>
-        <v>N</v>
-      </c>
-      <c r="AA2" s="1" t="str">
-        <f ca="1"/>
-        <v>Y</v>
-      </c>
-      <c r="AB2" s="1" t="str">
-        <f ca="1"/>
-        <v>Abi Gerçekten Çok güzel olmuş site</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="e" cm="1">
+        <f t="array" aca="1" ref="B2" ca="1">RIGHT(_xlfn.ANCHORARRAY(Insert!B2), LEN(_xlfn.ANCHORARRAY(Insert!B2)) - FIND("=",_xlfn.ANCHORARRAY( Insert!B2)))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
+      <c r="R2" s="1"/>
+      <c r="S2" s="1"/>
+      <c r="T2" s="1"/>
+      <c r="U2" s="1"/>
+      <c r="V2" s="1"/>
+      <c r="W2" s="1"/>
+      <c r="X2" s="1"/>
+      <c r="Y2" s="1"/>
+      <c r="Z2" s="1"/>
+      <c r="AA2" s="1"/>
+      <c r="AB2" s="1"/>
       <c r="AC2" s="1"/>
       <c r="AD2" s="4"/>
       <c r="AE2" s="4"/>
@@ -3599,7 +3363,7 @@
       <c r="AO2" s="4"/>
       <c r="AP2" s="4"/>
     </row>
-    <row r="3" spans="1:42">
+    <row r="3" spans="1:43">
       <c r="A3">
         <f>Insert!A3</f>
         <v>0</v>
@@ -3613,9 +3377,7 @@
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
-      <c r="H3" s="1">
-        <v>6</v>
-      </c>
+      <c r="H3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
@@ -3651,119 +3413,41 @@
       <c r="AO3" s="4"/>
       <c r="AP3" s="4"/>
     </row>
-    <row r="4" spans="1:42">
-      <c r="A4" t="str">
+    <row r="4" spans="1:43">
+      <c r="A4">
         <f>Insert!A4</f>
-        <v>s=Yiğit Emre Çulcuoğlu;e=2022 İzmir Regional;l=f;m=1;r=b2;t=6838;as=[54];at=Y;au=8;al=3;ac=Y;tu=5;tl=6;tm=1;tn=2;wd=Y;cl=b;ss=[53,56,44,58,34,20,17,18,41,51,51,16,26,50,64,68,34];c=4;be=Y;cn=1;ds=v;dr=v;d=N;to=N;cf=N;co=Commen</v>
-      </c>
-      <c r="B4" s="1" t="str" cm="1">
-        <f t="array" aca="1" ref="B4:AB4" ca="1">RIGHT(_xlfn.ANCHORARRAY(Insert!B4), LEN(_xlfn.ANCHORARRAY(Insert!B4)) - FIND("=",_xlfn.ANCHORARRAY( Insert!B4)))</f>
-        <v>Yiğit Emre Çulcuoğlu</v>
-      </c>
-      <c r="C4" s="1" t="str">
-        <f ca="1"/>
-        <v>2022 İzmir Regional</v>
-      </c>
-      <c r="D4" s="1" t="str">
-        <f ca="1"/>
-        <v>f</v>
-      </c>
-      <c r="E4" s="1" t="str">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="F4" s="1" t="str">
-        <f ca="1"/>
-        <v>b2</v>
-      </c>
-      <c r="G4" s="1" t="str">
-        <f ca="1"/>
-        <v>6838</v>
-      </c>
-      <c r="H4" s="1" t="str">
-        <f ca="1"/>
-        <v>[54]</v>
-      </c>
-      <c r="I4" s="1" t="str">
-        <f ca="1"/>
-        <v>Y</v>
-      </c>
-      <c r="J4" s="1" t="str">
-        <f ca="1"/>
-        <v>8</v>
-      </c>
-      <c r="K4" s="1" t="str">
-        <f ca="1"/>
-        <v>3</v>
-      </c>
-      <c r="L4" s="1" t="str">
-        <f ca="1"/>
-        <v>Y</v>
-      </c>
-      <c r="M4" s="1" t="str">
-        <f ca="1"/>
-        <v>5</v>
-      </c>
-      <c r="N4" s="1" t="str">
-        <f ca="1"/>
-        <v>6</v>
-      </c>
-      <c r="O4" s="1" t="str">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="P4" s="1" t="str">
-        <f ca="1"/>
-        <v>2</v>
-      </c>
-      <c r="Q4" s="1" t="str">
-        <f ca="1"/>
-        <v>Y</v>
-      </c>
-      <c r="R4" s="1" t="str">
-        <f ca="1"/>
-        <v>b</v>
-      </c>
-      <c r="S4" s="1" t="str">
-        <f ca="1"/>
-        <v>[53,56,44,58,34,20,17,18,41,51,51,16,26,50,64,68,34]</v>
-      </c>
-      <c r="T4" s="1" t="str">
-        <f ca="1"/>
-        <v>4</v>
-      </c>
-      <c r="U4" s="1" t="str">
-        <f ca="1"/>
-        <v>Y</v>
-      </c>
-      <c r="V4" s="1" t="str">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="W4" s="1" t="str">
-        <f ca="1"/>
-        <v>v</v>
-      </c>
-      <c r="X4" s="1" t="str">
-        <f ca="1"/>
-        <v>v</v>
-      </c>
-      <c r="Y4" s="1" t="str">
-        <f ca="1"/>
-        <v>N</v>
-      </c>
-      <c r="Z4" s="1" t="str">
-        <f ca="1"/>
-        <v>N</v>
-      </c>
-      <c r="AA4" s="1" t="str">
-        <f ca="1"/>
-        <v>N</v>
-      </c>
-      <c r="AB4" s="1" t="str">
-        <f ca="1"/>
-        <v>Commen</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="B4" s="1" t="e" cm="1">
+        <f t="array" aca="1" ref="B4" ca="1">RIGHT(_xlfn.ANCHORARRAY(Insert!B4), LEN(_xlfn.ANCHORARRAY(Insert!B4)) - FIND("=",_xlfn.ANCHORARRAY( Insert!B4)))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
+      <c r="Q4" s="1"/>
+      <c r="R4" s="1"/>
+      <c r="S4" s="1"/>
+      <c r="T4" s="1"/>
+      <c r="U4" s="1"/>
+      <c r="V4" s="1"/>
+      <c r="W4" s="1"/>
+      <c r="X4" s="1"/>
+      <c r="Y4" s="1"/>
+      <c r="Z4" s="1"/>
+      <c r="AA4" s="1"/>
+      <c r="AB4" s="1"/>
       <c r="AC4" s="1"/>
       <c r="AD4" s="4"/>
       <c r="AE4" s="4"/>
@@ -3779,7 +3463,7 @@
       <c r="AO4" s="4"/>
       <c r="AP4" s="4"/>
     </row>
-    <row r="5" spans="1:42">
+    <row r="5" spans="1:43">
       <c r="A5">
         <f>Insert!A5</f>
         <v>0</v>
@@ -3829,7 +3513,7 @@
       <c r="AO5" s="4"/>
       <c r="AP5" s="4"/>
     </row>
-    <row r="6" spans="1:42">
+    <row r="6" spans="1:43">
       <c r="A6">
         <f>Insert!A6</f>
         <v>0</v>
@@ -3879,7 +3563,7 @@
       <c r="AO6" s="4"/>
       <c r="AP6" s="4"/>
     </row>
-    <row r="7" spans="1:42">
+    <row r="7" spans="1:43">
       <c r="A7">
         <f>Insert!A7</f>
         <v>0</v>
@@ -3929,7 +3613,7 @@
       <c r="AO7" s="4"/>
       <c r="AP7" s="4"/>
     </row>
-    <row r="8" spans="1:42">
+    <row r="8" spans="1:43">
       <c r="A8">
         <f>Insert!A8</f>
         <v>0</v>
@@ -3979,7 +3663,7 @@
       <c r="AO8" s="4"/>
       <c r="AP8" s="4"/>
     </row>
-    <row r="9" spans="1:42">
+    <row r="9" spans="1:43">
       <c r="A9">
         <f>Insert!A9</f>
         <v>0</v>
@@ -4029,7 +3713,7 @@
       <c r="AO9" s="4"/>
       <c r="AP9" s="4"/>
     </row>
-    <row r="10" spans="1:42">
+    <row r="10" spans="1:43">
       <c r="A10">
         <f>Insert!A10</f>
         <v>0</v>
@@ -4079,7 +3763,7 @@
       <c r="AO10" s="4"/>
       <c r="AP10" s="4"/>
     </row>
-    <row r="11" spans="1:42">
+    <row r="11" spans="1:43">
       <c r="A11">
         <f>Insert!A11</f>
         <v>0</v>
@@ -4129,7 +3813,7 @@
       <c r="AO11" s="4"/>
       <c r="AP11" s="4"/>
     </row>
-    <row r="12" spans="1:42">
+    <row r="12" spans="1:43">
       <c r="A12">
         <f>Insert!A12</f>
         <v>0</v>
@@ -4179,7 +3863,7 @@
       <c r="AO12" s="4"/>
       <c r="AP12" s="4"/>
     </row>
-    <row r="13" spans="1:42">
+    <row r="13" spans="1:43">
       <c r="A13">
         <f>Insert!A13</f>
         <v>0</v>
@@ -4229,7 +3913,7 @@
       <c r="AO13" s="4"/>
       <c r="AP13" s="4"/>
     </row>
-    <row r="14" spans="1:42">
+    <row r="14" spans="1:43">
       <c r="A14">
         <f>Insert!A14</f>
         <v>0</v>
@@ -4279,7 +3963,7 @@
       <c r="AO14" s="4"/>
       <c r="AP14" s="4"/>
     </row>
-    <row r="15" spans="1:42">
+    <row r="15" spans="1:43">
       <c r="A15">
         <f>Insert!A15</f>
         <v>0</v>
@@ -4329,7 +4013,7 @@
       <c r="AO15" s="4"/>
       <c r="AP15" s="4"/>
     </row>
-    <row r="16" spans="1:42">
+    <row r="16" spans="1:43">
       <c r="A16">
         <f>Insert!A16</f>
         <v>0</v>

</xml_diff>